<commit_message>
FRE nav & shoppingcart
</commit_message>
<xml_diff>
--- a/_Adminstratives/Frontend/Statische Seite_Aufteilung Umsetzung.xlsx
+++ b/_Adminstratives/Frontend/Statische Seite_Aufteilung Umsetzung.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chris\_Daten\5_Fortbildung\517 Junior SWE (2025)\Projekt\In-crust-we-trust\_Adminstratives\Frontend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02E36368-C426-4244-988F-8828B6FE458D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEFC9E78-9964-4F8D-8170-BAE05C6F4A7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{9A469A0A-967A-4A25-80A5-4F5EDB201578}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="44">
   <si>
     <t>Footer</t>
   </si>
@@ -545,7 +545,7 @@
   <dimension ref="A1:D27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -573,6 +573,9 @@
       <c r="C2" t="s">
         <v>10</v>
       </c>
+      <c r="D2" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
@@ -602,8 +605,11 @@
       <c r="C5" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -658,6 +664,9 @@
       </c>
       <c r="C10" t="s">
         <v>10</v>
+      </c>
+      <c r="D10" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
FRE static sites CPF finished
</commit_message>
<xml_diff>
--- a/_Adminstratives/Frontend/Statische Seite_Aufteilung Umsetzung.xlsx
+++ b/_Adminstratives/Frontend/Statische Seite_Aufteilung Umsetzung.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28827"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\christian.pfneisl\Desktop\_FH\517-Junior-SWE-2025\Projekt\In-crust-we-trust\_Adminstratives\Frontend\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF72F978-DED9-4FB8-8E7C-CB2F63F059D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet r:id="rId1" sheetId="1" name="Tabelle1"/>
+    <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="45">
   <si>
     <t>Anm./ Todos</t>
   </si>
@@ -146,14 +152,16 @@
   </si>
   <si>
     <t>Navbar über Script einbinden</t>
+  </si>
+  <si>
+    <t>Seite</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -162,10 +170,25 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
+      <sz val="8"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -176,7 +199,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -191,39 +214,44 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+  <cellXfs count="6">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" builtinId="0" name="Normal"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -234,10 +262,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="0E2841"/>
@@ -275,71 +303,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Times New Roman" script="Arab"/>
-        <a:font typeface="Times New Roman" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="MoolBoran" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Times New Roman" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Arial" script="Arab"/>
-        <a:font typeface="Arial" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="DaunPenh" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Arial" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -367,7 +395,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -390,11 +418,11 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="9500"/>
@@ -403,13 +431,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -419,7 +447,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -428,7 +456,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -437,7 +465,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -445,10 +473,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot rev="0" lon="0" lat="0"/>
+              <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
-              <a:rot rev="1200000" lon="0" lat="0"/>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -513,37 +541,42 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:D27"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" style="5" width="33.86214285714286" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="6" width="61.57642857142857" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="5" width="13.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="33.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="61.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
-      <c r="A1" s="1"/>
-      <c r="B1" s="2" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1" t="s">
+      <c r="C1" s="4"/>
+      <c r="D1" s="4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75" customFormat="1" s="3">
+    <row r="2" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C2" s="2" t="s">
@@ -553,33 +586,31 @@
         <v>5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75" customFormat="1" s="3">
+    <row r="3" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="2"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75" customFormat="1" s="3">
+    </row>
+    <row r="4" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="4"/>
+      <c r="B4" s="3"/>
       <c r="C4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="2"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75" customFormat="1" s="3">
+    </row>
+    <row r="5" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="4"/>
+      <c r="B5" s="3"/>
       <c r="C5" s="2" t="s">
         <v>4</v>
       </c>
@@ -587,23 +618,22 @@
         <v>5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="32.25" customFormat="1" s="3">
+    <row r="6" spans="1:4" s="2" customFormat="1" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="3" t="s">
         <v>12</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="2"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75" customFormat="1" s="3">
+    </row>
+    <row r="7" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="4"/>
+      <c r="B7" s="3"/>
       <c r="C7" s="2" t="s">
         <v>4</v>
       </c>
@@ -611,23 +641,22 @@
         <v>5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75" customFormat="1" s="3">
+    <row r="8" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="3" t="s">
         <v>15</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D8" s="2"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75" customFormat="1" s="3">
+    </row>
+    <row r="9" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="4"/>
+      <c r="B9" s="3"/>
       <c r="C9" s="2" t="s">
         <v>4</v>
       </c>
@@ -635,11 +664,11 @@
         <v>5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="32.25" customFormat="1" s="3">
+    <row r="10" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="3" t="s">
         <v>18</v>
       </c>
       <c r="C10" s="2" t="s">
@@ -649,11 +678,11 @@
         <v>5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75" customFormat="1" s="3">
+    <row r="11" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B11" s="4"/>
+      <c r="B11" s="3"/>
       <c r="C11" s="2" t="s">
         <v>4</v>
       </c>
@@ -661,47 +690,44 @@
         <v>5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75" customFormat="1" s="3">
+    <row r="12" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="3" t="s">
         <v>21</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D12" s="2"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="32.25" customFormat="1" s="3">
+    </row>
+    <row r="13" spans="1:4" s="2" customFormat="1" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B13" s="3" t="s">
         <v>23</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D13" s="2"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75" customFormat="1" s="3">
+    </row>
+    <row r="14" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="3" t="s">
         <v>25</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D14" s="2"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75" customFormat="1" s="3">
+    </row>
+    <row r="15" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B15" s="3" t="s">
         <v>27</v>
       </c>
       <c r="C15" s="2" t="s">
@@ -711,11 +737,11 @@
         <v>5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="32.25" customFormat="1" s="3">
+    <row r="16" spans="1:4" s="2" customFormat="1" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B16" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C16" s="2" t="s">
@@ -725,11 +751,11 @@
         <v>5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="32.25" customFormat="1" s="3">
+    <row r="17" spans="1:4" s="2" customFormat="1" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="B17" s="3" t="s">
         <v>32</v>
       </c>
       <c r="C17" s="2" t="s">
@@ -739,25 +765,21 @@
         <v>5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="32.25" customFormat="1" s="3">
+    <row r="18" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="B18" s="3" t="s">
         <v>34</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="D18" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B19" s="2"/>
       <c r="C19" s="1" t="s">
         <v>4</v>
       </c>
@@ -765,11 +787,10 @@
         <v>5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B20" s="2"/>
       <c r="C20" s="1" t="s">
         <v>4</v>
       </c>
@@ -777,11 +798,10 @@
         <v>5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B21" s="2"/>
       <c r="C21" s="1" t="s">
         <v>4</v>
       </c>
@@ -789,11 +809,10 @@
         <v>5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B22" s="2"/>
       <c r="C22" s="1" t="s">
         <v>4</v>
       </c>
@@ -801,11 +820,10 @@
         <v>5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18.75">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B23" s="2"/>
       <c r="C23" s="1" t="s">
         <v>4</v>
       </c>
@@ -813,7 +831,7 @@
         <v>5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18.75">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>40</v>
       </c>
@@ -823,31 +841,19 @@
       <c r="C24" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D24" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75">
-      <c r="A25" s="1"/>
-      <c r="B25" s="2"/>
-      <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18.75">
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B26" s="2"/>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="18.75">
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B27" s="2"/>
-      <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
BAE: started putting data into DB
</commit_message>
<xml_diff>
--- a/_Adminstratives/Frontend/Statische Seite_Aufteilung Umsetzung.xlsx
+++ b/_Adminstratives/Frontend/Statische Seite_Aufteilung Umsetzung.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\christian.pfneisl\Desktop\_FH\517-Junior-SWE-2025\Projekt\In-crust-we-trust\_Adminstratives\Frontend\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chris\_Daten\5_Fortbildung\517 Junior SWE (2025)\Projekt\In-crust-we-trust\_Adminstratives\Frontend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF72F978-DED9-4FB8-8E7C-CB2F63F059D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED1629C3-DBD9-40FE-AE95-31F4E31E35ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -88,12 +88,6 @@
     <t>PLZ / Ort tauschen;  Bestelldetails ev. an Design Warenkorb anpassen</t>
   </si>
   <si>
-    <t>Checkout - Bestellung - Adminansicht</t>
-  </si>
-  <si>
-    <t>Seite verdoppeln und anpassen - kein Bestellbutton, zuzätzlich Lieferdatum (siehe Produktadmin)</t>
-  </si>
-  <si>
     <t>Sweetalert Bestellbestätigung</t>
   </si>
   <si>
@@ -155,6 +149,12 @@
   </si>
   <si>
     <t>Seite</t>
+  </si>
+  <si>
+    <t>Bestellung - Detailansicht (Basis ist der Checkout-Siete)</t>
+  </si>
+  <si>
+    <t>Checkouts Seite verdoppeln und anpassen - kein Bestellbutton, zuzätzlich Lieferdatum (siehe Produktadmin)</t>
   </si>
 </sst>
 </file>
@@ -548,21 +548,21 @@
   <dimension ref="A1:D27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="10.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="33.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="61.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="33.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="68.54296875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="13.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>0</v>
@@ -572,7 +572,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -586,7 +586,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -597,7 +597,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>9</v>
       </c>
@@ -606,7 +606,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>10</v>
       </c>
@@ -618,7 +618,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:4" s="2" customFormat="1" ht="22.5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>11</v>
       </c>
@@ -629,7 +629,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>13</v>
       </c>
@@ -641,7 +641,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>14</v>
       </c>
@@ -652,7 +652,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>16</v>
       </c>
@@ -664,7 +664,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>17</v>
       </c>
@@ -678,7 +678,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>19</v>
       </c>
@@ -690,7 +690,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>20</v>
       </c>
@@ -701,7 +701,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:4" s="2" customFormat="1" ht="22.5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>22</v>
       </c>
@@ -712,7 +712,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>24</v>
       </c>
@@ -720,24 +720,27 @@
         <v>25</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.2">
+        <v>26</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C15" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B15" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>28</v>
-      </c>
       <c r="D15" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:4" s="2" customFormat="1" ht="22.5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" s="2" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>29</v>
       </c>
@@ -745,13 +748,13 @@
         <v>30</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:4" s="2" customFormat="1" ht="22.5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>31</v>
       </c>
@@ -759,97 +762,94 @@
         <v>32</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="C18" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C18" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" s="1" t="s">
+      <c r="C19" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C19" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" s="1" t="s">
+      <c r="C20" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C20" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" s="1" t="s">
+      <c r="C21" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C21" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" s="1" t="s">
+      <c r="C22" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" s="2" customFormat="1" ht="21" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C22" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" s="1" t="s">
+      <c r="B24" s="2" t="s">
         <v>39</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>41</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>